<commit_message>
update 004EMP et maj
</commit_message>
<xml_diff>
--- a/TNR_JDD/TNRSequencer.xlsx
+++ b/TNR_JDD/TNRSequencer.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
   <si>
     <t>CAS_DE_TEST</t>
   </si>
@@ -80,6 +80,12 @@
   </si>
   <si>
     <t>RO.ACT.004EMP.SRM</t>
+  </si>
+  <si>
+    <t>RO.ACT.004</t>
+  </si>
+  <si>
+    <t>RO.ACT.003</t>
   </si>
 </sst>
 </file>
@@ -431,7 +437,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -476,7 +482,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
@@ -495,6 +501,9 @@
       </c>
     </row>
     <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
       <c r="D4" t="s">
         <v>5</v>
       </c>
@@ -512,6 +521,9 @@
       </c>
     </row>
     <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
       <c r="D5" t="s">
         <v>3</v>
       </c>
@@ -528,22 +540,39 @@
         <v>21</v>
       </c>
     </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="8" spans="1:8">
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
       <c r="E8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:8">
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
       <c r="E9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:8">
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
       <c r="E10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:8">
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
       <c r="E11" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Update KW et Tools
KW Ajout de GlobalVariable.TIMEOUTForPageLoad = 5 sec
KW Ajout de waitForPageLoad() dans openBrowser()
KWAjout de waitForPageLoad() dans navigateToUrl()
Tools getBrowserAndVersion ajout DriverFactory.getExecutedBrowser()
KW ajout deay() dans scrollAndClick et scrollAndDoubleClick
TC ajout de delay dans les TC HAB.SRM et MET.SRM
TC waitForElementVisible prise en compte du retour TRUE/FASE
</commit_message>
<xml_diff>
--- a/TNR_JDD/TNRSequencer.xlsx
+++ b/TNR_JDD/TNRSequencer.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>CAS_DE_TEST</t>
   </si>
@@ -445,7 +445,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:B13"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -469,7 +469,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>20</v>
@@ -488,8 +488,11 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>2</v>
@@ -508,9 +511,7 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="A4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>21</v>
       </c>
@@ -528,9 +529,7 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="A5" s="2"/>
       <c r="D5" t="s">
         <v>19</v>
       </c>
@@ -548,9 +547,6 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
       <c r="E6" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
feat Log Result PREJDDFiles TCFiles Test Listeners
Log : Create folder if not exist
PREJDDFiles : Create folder if not exist
Result : Create folder if not exist
Result.addStep : update 
TCFiles : add getTCNameTitle and getAutoTitle
Log.addStartTestCase : add getTCNameTitle
Log.addSTEPERROR : add this.status.ERROR++
</commit_message>
<xml_diff>
--- a/TNR_JDD/TNRSequencer.xlsx
+++ b/TNR_JDD/TNRSequencer.xlsx
@@ -448,7 +448,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B15:B16"/>
+      <selection activeCell="I21" sqref="H18:I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -492,7 +492,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Add STEPACTION and rename addSTEPSSGRP en addSTEPBLOCK
Log.addSTEPACTION
Result : cellStyle_RESULT_STEPACTION
</commit_message>
<xml_diff>
--- a/TNR_JDD/TNRSequencer.xlsx
+++ b/TNR_JDD/TNRSequencer.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>CAS_DE_TEST</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>AD.SEC.001.FON.99</t>
+  </si>
+  <si>
+    <t>ZZ.010</t>
   </si>
 </sst>
 </file>
@@ -449,7 +452,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -473,21 +476,14 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="2"/>
+      <c r="A3" s="2"/>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2"/>
@@ -550,7 +546,7 @@
   <dimension ref="B2:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Ajout dossier dans TNR_Result
</commit_message>
<xml_diff>
--- a/TNR_JDD/TNRSequencer.xlsx
+++ b/TNR_JDD/TNRSequencer.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>CAS_DE_TEST</t>
   </si>
@@ -449,7 +449,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -477,24 +477,13 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A3" s="2"/>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="A4" s="2"/>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
+      <c r="A5" s="2"/>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2"/>

</xml_diff>